<commit_message>
2023.9.21 precode check 0.1.5 实现precode和适用项目的检查
</commit_message>
<xml_diff>
--- a/check_precode/用例列表.xlsx
+++ b/check_precode/用例列表.xlsx
@@ -163,7 +163,7 @@
     <t>LIAI-13676,LIAI-14787</t>
   </si>
   <si>
-    <t>语音环境_继电器,X平台,语音Xpublic,语音环境</t>
+    <t>语音环境_继电器,X平台,语音Xm,语音环境</t>
   </si>
   <si>
     <t>X01_语音_交互框架_358724_网络良好可完成声纹注册流程</t>
@@ -337,6 +337,9 @@
     <t>362730</t>
   </si>
   <si>
+    <t>X-Public-Pro</t>
+  </si>
+  <si>
     <t>语音_百科/问答/闲聊_195263</t>
   </si>
   <si>
@@ -377,9 +380,6 @@
   </si>
   <si>
     <t>195263</t>
-  </si>
-  <si>
-    <t>X-Public-Pro</t>
   </si>
   <si>
     <t>语音_得到_423367</t>
@@ -1217,7 +1217,7 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1365,15 +1365,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1910,1722 +1916,1724 @@
   <sheetPr/>
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AE12" sqref="A1:AE18"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="31" width="16.716814159292" customWidth="1"/>
+    <col min="1" max="24" width="16.716814159292" customWidth="1"/>
+    <col min="25" max="25" width="61.5575221238938" style="1" customWidth="1"/>
+    <col min="26" max="31" width="16.716814159292" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1" spans="1:31">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:31">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="2" t="s">
+      <c r="R2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" s="2" t="s">
+      <c r="U2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AA2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:31">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="M3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="2" t="s">
+      <c r="R3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="2" t="s">
+      <c r="U3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="Z3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AA3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AA3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AE3" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:31">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="M4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" s="2" t="s">
+      <c r="R4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y4" s="2" t="s">
+      <c r="U4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="Z4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AA4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AA4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AE4" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:31">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="2" t="s">
+      <c r="M5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S5" s="2" t="s">
+      <c r="R5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="U5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y5" s="2" t="s">
+      <c r="U5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="Z5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AA5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AA5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AE5" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:31">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="2" t="s">
+      <c r="M6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S6" s="2" t="s">
+      <c r="R6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="U6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y6" s="2" t="s">
+      <c r="U6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="Z6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AA6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AA6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AE6" s="2" t="s">
-        <v>68</v>
+      <c r="AE6" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:31">
-      <c r="A7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="K7" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="2" t="s">
+      <c r="L7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q7" s="2" t="s">
+      <c r="P7" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S7" s="2" t="s">
+      <c r="R7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="T7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="U7" s="2" t="s">
+      <c r="T7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="V7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y7" s="2" t="s">
+      <c r="U7" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="V7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AA7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD7" s="2" t="s">
+      <c r="Z7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="AE7" s="2" t="s">
+      <c r="AA7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD7" s="3" t="s">
         <v>117</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:31">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N8" s="2" t="s">
+      <c r="M8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S8" s="2" t="s">
+      <c r="R8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T8" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="U8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y8" s="2" t="s">
+      <c r="U8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="Z8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="AA8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AA8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD8" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AE8" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:31">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N9" s="2" t="s">
+      <c r="M9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S9" s="2" t="s">
+      <c r="R9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="U9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y9" s="2" t="s">
+      <c r="U9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y9" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Z9" s="2" t="s">
+      <c r="Z9" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="AA9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AA9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD9" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="AE9" s="2" t="s">
+      <c r="AE9" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:31">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="2" t="s">
+      <c r="M10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S10" s="2" t="s">
+      <c r="R10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="T10" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="U10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y10" s="2" t="s">
+      <c r="U10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y10" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="Z10" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AA10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD10" s="2" t="s">
+      <c r="AA10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD10" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="AE10" s="2" t="s">
-        <v>68</v>
+      <c r="AE10" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:31">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N11" s="2" t="s">
+      <c r="M11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P11" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S11" s="2" t="s">
+      <c r="R11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="T11" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="U11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y11" s="2" t="s">
+      <c r="U11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Z11" s="2" t="s">
+      <c r="Z11" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="AA11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AA11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD11" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="AE11" s="2" t="s">
+      <c r="AE11" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:31">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" s="2" t="s">
+      <c r="M12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S12" s="2" t="s">
+      <c r="R12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="T12" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="U12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y12" s="2" t="s">
+      <c r="U12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Z12" s="2" t="s">
+      <c r="Z12" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="AA12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD12" s="2" t="s">
+      <c r="AA12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD12" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="AE12" s="2" t="s">
+      <c r="AE12" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:31">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="M13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="2" t="s">
+      <c r="M13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q13" s="2" t="s">
+      <c r="P13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S13" s="2" t="s">
+      <c r="R13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="T13" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="U13" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="V13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y13" s="2" t="s">
+      <c r="V13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y13" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="Z13" s="2" t="s">
+      <c r="Z13" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="AA13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AA13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD13" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="AE13" s="2" t="s">
+      <c r="AE13" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:31">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N14" s="2" t="s">
+      <c r="M14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P14" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S14" s="2" t="s">
+      <c r="R14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="T14" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="U14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y14" s="2" t="s">
+      <c r="U14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y14" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="Z14" s="2" t="s">
+      <c r="Z14" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AA14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD14" s="2" t="s">
+      <c r="AA14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD14" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AE14" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:31">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" s="2" t="s">
+      <c r="M15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="P15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="Q15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S15" s="2" t="s">
+      <c r="R15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T15" s="2" t="s">
+      <c r="T15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="U15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y15" s="2" t="s">
+      <c r="U15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="2" t="s">
+      <c r="Z15" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="AA15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AA15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD15" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="AE15" s="2" t="s">
-        <v>68</v>
+      <c r="AE15" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" ht="14" customHeight="1" spans="1:31">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" s="2" t="s">
+      <c r="M16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="Q16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S16" s="2" t="s">
+      <c r="R16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T16" s="2" t="s">
+      <c r="T16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="U16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y16" s="2" t="s">
+      <c r="U16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Z16" s="2" t="s">
+      <c r="Z16" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="AA16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AA16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD16" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="AE16" s="2" t="s">
+      <c r="AE16" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="17" ht="14" customHeight="1" spans="1:31">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="M17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" s="2" t="s">
+      <c r="M17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q17" s="2" t="s">
+      <c r="P17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S17" s="2" t="s">
+      <c r="R17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="T17" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="U17" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="V17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y17" s="2" t="s">
+      <c r="V17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y17" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="Z17" s="2" t="s">
+      <c r="Z17" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AA17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AA17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD17" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="AE17" s="2" t="s">
+      <c r="AE17" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" ht="14" customHeight="1" spans="1:31">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="D18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="M18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N18" s="2" t="s">
+      <c r="M18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q18" s="2" t="s">
+      <c r="P18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S18" s="2" t="s">
+      <c r="R18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S18" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="T18" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="U18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y18" s="2" t="s">
+      <c r="U18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y18" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="Z18" s="2" t="s">
+      <c r="Z18" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="AA18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD18" s="2" t="s">
+      <c r="AA18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD18" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="AE18" s="2" t="s">
+      <c r="AE18" s="3" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>